<commit_message>
Finalizes all main functionalities of the applicatoins. Several TODOs and  testing are pedning.
</commit_message>
<xml_diff>
--- a/inquiries/Minerva_ATACseq/Bulk Storage_Report_ATACseq_PBMC.xlsx
+++ b/inquiries/Minerva_ATACseq/Bulk Storage_Report_ATACseq_PBMC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MounSinai\Darpa\Programming\DownloadRequestCreator\inquiries\Minerva_ATACseq\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F5B05E-7643-42FF-9B16-CA607C0AB3CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F2DFCF-0DE7-4525-A876-6B3491AF1BC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30840" yWindow="5295" windowWidth="16035" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5184" yWindow="1932" windowWidth="16032" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bulk Storage_Report_RNAseq_PBMC" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
   <si>
     <t>Type</t>
   </si>
@@ -66,6 +66,24 @@
   </si>
   <si>
     <t>ATACseq_4</t>
+  </si>
+  <si>
+    <t>STAS-06412_4</t>
+  </si>
+  <si>
+    <t>RNAseq</t>
+  </si>
+  <si>
+    <t>FS07-06412_3</t>
+  </si>
+  <si>
+    <t>FS07-06412</t>
+  </si>
+  <si>
+    <t>FS07-05884_3</t>
+  </si>
+  <si>
+    <t>FS07-05884</t>
   </si>
 </sst>
 </file>
@@ -97,12 +115,22 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBDBDBD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE7F5E9"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -117,13 +145,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -443,10 +480,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="A5" sqref="A5:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -524,6 +561,75 @@
       </c>
       <c r="G3" s="3" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adds functionality to run external process (Data Downloader) based on configuration settings. Moves data_source config files to 'configs' subfolders inside of each data source.
</commit_message>
<xml_diff>
--- a/inquiries/Minerva_ATACseq/Bulk Storage_Report_ATACseq_PBMC.xlsx
+++ b/inquiries/Minerva_ATACseq/Bulk Storage_Report_ATACseq_PBMC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MounSinai\Darpa\Programming\DownloadRequestCreator\inquiries\Minerva_ATACseq\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F2DFCF-0DE7-4525-A876-6B3491AF1BC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F5B05E-7643-42FF-9B16-CA607C0AB3CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5184" yWindow="1932" windowWidth="16032" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30840" yWindow="5295" windowWidth="16035" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bulk Storage_Report_RNAseq_PBMC" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>Type</t>
   </si>
@@ -66,24 +66,6 @@
   </si>
   <si>
     <t>ATACseq_4</t>
-  </si>
-  <si>
-    <t>STAS-06412_4</t>
-  </si>
-  <si>
-    <t>RNAseq</t>
-  </si>
-  <si>
-    <t>FS07-06412_3</t>
-  </si>
-  <si>
-    <t>FS07-06412</t>
-  </si>
-  <si>
-    <t>FS07-05884_3</t>
-  </si>
-  <si>
-    <t>FS07-05884</t>
   </si>
 </sst>
 </file>
@@ -115,22 +97,12 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFBDBDBD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE7F5E9"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -145,22 +117,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -480,10 +443,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:G6"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -561,75 +524,6 @@
       </c>
       <c r="G3" s="3" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>